<commit_message>
Scenarios and memberships updated
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Scenario</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Taco bell</t>
   </si>
 </sst>
 </file>
@@ -645,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N18"/>
+  <dimension ref="B1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +726,7 @@
         <v>41182</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="b">
         <v>1</v>
@@ -746,99 +749,76 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="7">
         <v>41296</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="7">
         <v>40817</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="7">
         <v>41182</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="3" t="b">
+      <c r="H7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
         <v>41061</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K7" s="7">
         <v>41292</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6">
+      <c r="L7" s="7"/>
+      <c r="M7">
         <v>3</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-    </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E8" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F8" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>41244</v>
-      </c>
-      <c r="K8" s="7">
-        <v>41292</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8">
-        <v>2</v>
-      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="7">
         <v>41296</v>
@@ -850,74 +830,72 @@
         <v>41182</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="7">
-        <v>41000</v>
+        <v>41244</v>
       </c>
       <c r="K9" s="7">
-        <v>41264</v>
+        <v>41292</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E10" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F10" s="7">
+        <v>41182</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <v>41000</v>
+      </c>
+      <c r="K10" s="7">
+        <v>41264</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E11" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F11" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>41214</v>
-      </c>
-      <c r="K11" s="7">
-        <v>41292</v>
-      </c>
-      <c r="L11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>4</v>
-      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="7">
         <v>41296</v>
@@ -929,63 +907,63 @@
         <v>41182</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>41214</v>
+      </c>
+      <c r="K12" s="7">
+        <v>41292</v>
+      </c>
+      <c r="L12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E13" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F13" s="7">
+        <v>41182</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="3" t="b">
+      <c r="H13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7">
+      <c r="I13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
         <v>41000</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K13" s="7">
         <v>41203</v>
       </c>
-      <c r="L12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12">
+      <c r="L13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E15" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F15" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <v>41214</v>
-      </c>
-      <c r="K15" s="7">
-        <v>41292</v>
-      </c>
-      <c r="L15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -993,7 +971,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D16" s="7">
         <v>41296</v>
@@ -1005,7 +983,7 @@
         <v>41182</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="3" t="b">
         <v>0</v>
@@ -1014,22 +992,25 @@
         <v>0</v>
       </c>
       <c r="J16" s="7">
-        <v>41000</v>
+        <v>41214</v>
       </c>
       <c r="K16" s="7">
-        <v>41203</v>
+        <v>41292</v>
       </c>
       <c r="L16" s="7" t="b">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="7">
         <v>41296</v>
       </c>
@@ -1040,7 +1021,7 @@
         <v>41182</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="b">
         <v>0</v>
@@ -1049,25 +1030,22 @@
         <v>0</v>
       </c>
       <c r="J17" s="7">
-        <v>40831</v>
+        <v>41000</v>
       </c>
       <c r="K17" s="7">
-        <v>40923</v>
+        <v>41203</v>
       </c>
       <c r="L17" s="7" t="b">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
       <c r="D18" s="7">
         <v>41296</v>
       </c>
@@ -1078,16 +1056,16 @@
         <v>41182</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="7">
-        <v>40466</v>
+        <v>40831</v>
       </c>
       <c r="K18" s="7">
         <v>40923</v>
@@ -1096,6 +1074,44 @@
         <v>0</v>
       </c>
       <c r="M18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E19" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F19" s="7">
+        <v>41182</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>40466</v>
+      </c>
+      <c r="K19" s="7">
+        <v>40923</v>
+      </c>
+      <c r="L19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
This mornings integration changes
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Scenario</t>
   </si>
@@ -225,9 +225,6 @@
     <t>P27</t>
   </si>
   <si>
-    <t>S008</t>
-  </si>
-  <si>
     <t>P21</t>
   </si>
   <si>
@@ -264,6 +261,18 @@
   </si>
   <si>
     <t>Taco bell</t>
+  </si>
+  <si>
+    <t>Catg</t>
+  </si>
+  <si>
+    <t>MRE</t>
+  </si>
+  <si>
+    <t>NMR</t>
+  </si>
+  <si>
+    <t>S026</t>
   </si>
 </sst>
 </file>
@@ -648,27 +657,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N19"/>
+  <dimension ref="B1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5546875" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:14" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -676,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -687,29 +698,32 @@
       <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -726,29 +740,30 @@
         <v>41182</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>41061</v>
+      </c>
+      <c r="J5" s="7">
+        <v>41292</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>41061</v>
-      </c>
-      <c r="K5" s="7">
-        <v>41292</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="N5" s="3"/>
+      <c r="O5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
@@ -756,12 +771,13 @@
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
@@ -781,26 +797,27 @@
         <v>5</v>
       </c>
       <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>41061</v>
+      </c>
+      <c r="J7" s="7">
+        <v>41292</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>41061</v>
-      </c>
-      <c r="K7" s="7">
-        <v>41292</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="N7" s="3"/>
+      <c r="O7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="7"/>
@@ -808,12 +825,13 @@
       <c r="F8" s="7"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
@@ -835,21 +853,22 @@
       <c r="H9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="3" t="b">
-        <v>0</v>
+      <c r="I9" s="7">
+        <v>41244</v>
       </c>
       <c r="J9" s="7">
-        <v>41244</v>
-      </c>
-      <c r="K9" s="7">
         <v>41292</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9">
+      <c r="K9" s="7"/>
+      <c r="L9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
@@ -871,31 +890,32 @@
       <c r="H10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="3" t="b">
+      <c r="I10" s="7">
+        <v>41000</v>
+      </c>
+      <c r="J10" s="7">
+        <v>41264</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="7">
-        <v>41000</v>
-      </c>
-      <c r="K10" s="7">
-        <v>41264</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D12" s="7">
         <v>41296</v>
@@ -907,33 +927,36 @@
         <v>41182</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="3" t="b">
-        <v>0</v>
+      <c r="I12" s="7">
+        <v>41214</v>
       </c>
       <c r="J12" s="7">
-        <v>41214</v>
-      </c>
-      <c r="K12" s="7">
         <v>41292</v>
       </c>
-      <c r="L12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12">
+      <c r="K12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="7">
         <v>41296</v>
@@ -945,33 +968,36 @@
         <v>41182</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>41000</v>
+      </c>
+      <c r="J13" s="7">
+        <v>41203</v>
+      </c>
+      <c r="K13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7">
-        <v>41000</v>
-      </c>
-      <c r="K13" s="7">
-        <v>41203</v>
-      </c>
-      <c r="L13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="7">
         <v>41296</v>
@@ -983,33 +1009,34 @@
         <v>41182</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="3" t="b">
-        <v>0</v>
+      <c r="I16" s="7">
+        <v>41214</v>
       </c>
       <c r="J16" s="7">
-        <v>41214</v>
-      </c>
-      <c r="K16" s="7">
         <v>41292</v>
       </c>
-      <c r="L16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16">
+      <c r="K16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>41296</v>
@@ -1021,30 +1048,31 @@
         <v>41182</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="3" t="b">
-        <v>0</v>
+      <c r="I17" s="7">
+        <v>41000</v>
       </c>
       <c r="J17" s="7">
-        <v>41000</v>
-      </c>
-      <c r="K17" s="7">
         <v>41203</v>
       </c>
-      <c r="L17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17">
+      <c r="K17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="7">
         <v>41296</v>
@@ -1056,33 +1084,34 @@
         <v>41182</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="3" t="b">
-        <v>0</v>
+      <c r="I18" s="7">
+        <v>40831</v>
       </c>
       <c r="J18" s="7">
-        <v>40831</v>
-      </c>
-      <c r="K18" s="7">
         <v>40923</v>
       </c>
-      <c r="L18" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="K18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
       </c>
       <c r="D19" s="7">
         <v>41296</v>
@@ -1094,26 +1123,27 @@
         <v>41182</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
+        <v>40466</v>
+      </c>
+      <c r="J19" s="7">
+        <v>40923</v>
+      </c>
+      <c r="K19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7">
-        <v>40466</v>
-      </c>
-      <c r="K19" s="7">
-        <v>40923</v>
-      </c>
-      <c r="L19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>4</v>
-      </c>
+      <c r="N19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integration changes to FC mostly
Added some new flows and screens
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -66,8 +66,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Maps to the Unique Employment Pattern (Profile)
-</t>
+Asserted Override Date
+Enables a consistent result as time passes</t>
         </r>
       </text>
     </comment>
@@ -91,36 +91,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Asserted Override Date
-Enables a consistent result as time passes</t>
+Base Period Start Date</t>
         </r>
       </text>
     </comment>
     <comment ref="E3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Base Period Start Date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Scenario</t>
   </si>
@@ -159,12 +134,6 @@
   </si>
   <si>
     <t>Employer</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>P01</t>
   </si>
   <si>
     <t>Sams</t>
@@ -213,66 +182,48 @@
     <t>S006</t>
   </si>
   <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>P22</t>
-  </si>
-  <si>
     <t>Loews</t>
   </si>
   <si>
-    <t>P27</t>
-  </si>
-  <si>
-    <t>P21</t>
-  </si>
-  <si>
-    <t>P29</t>
-  </si>
-  <si>
     <t>Acme</t>
   </si>
   <si>
     <t>Wiley's</t>
   </si>
   <si>
-    <t>Asserted
+    <t>SFCD</t>
+  </si>
+  <si>
+    <t>Extra1</t>
+  </si>
+  <si>
+    <t>Extra2</t>
+  </si>
+  <si>
+    <t>S?</t>
+  </si>
+  <si>
+    <t>Taco bell</t>
+  </si>
+  <si>
+    <t>Catg</t>
+  </si>
+  <si>
+    <t>MRE</t>
+  </si>
+  <si>
+    <t>NMR</t>
+  </si>
+  <si>
+    <t>S026</t>
+  </si>
+  <si>
+    <t>Macy's</t>
+  </si>
+  <si>
+    <t>Asserted or Effective
 Process
 Date</t>
-  </si>
-  <si>
-    <t>SFCD</t>
-  </si>
-  <si>
-    <t>Extra1</t>
-  </si>
-  <si>
-    <t>Extra2</t>
-  </si>
-  <si>
-    <t>S?</t>
-  </si>
-  <si>
-    <t>P51</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Taco bell</t>
-  </si>
-  <si>
-    <t>Catg</t>
-  </si>
-  <si>
-    <t>MRE</t>
-  </si>
-  <si>
-    <t>NMR</t>
-  </si>
-  <si>
-    <t>S026</t>
   </si>
 </sst>
 </file>
@@ -657,493 +608,513 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O19"/>
+  <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" customWidth="1"/>
-    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" customWidth="1"/>
+    <col min="13" max="13" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:15" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:14" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
+      <c r="C5" s="7">
+        <v>41296</v>
       </c>
       <c r="D5" s="7">
-        <v>41296</v>
+        <v>40817</v>
       </c>
       <c r="E5" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F5" s="7">
         <v>41182</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="3" t="b">
-        <v>0</v>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>41061</v>
       </c>
       <c r="I5" s="7">
-        <v>41061</v>
-      </c>
-      <c r="J5" s="7">
         <v>41292</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5">
+      <c r="J5" s="7"/>
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="M5" s="3" t="b">
+      <c r="L5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M5" s="3"/>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="7">
+        <v>41296</v>
       </c>
       <c r="D7" s="7">
-        <v>41296</v>
+        <v>40817</v>
       </c>
       <c r="E7" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F7" s="7">
         <v>41182</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="b">
-        <v>0</v>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>41061</v>
       </c>
       <c r="I7" s="7">
-        <v>41061</v>
-      </c>
-      <c r="J7" s="7">
         <v>41292</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7">
+      <c r="J7" s="7"/>
+      <c r="K7">
         <v>3</v>
       </c>
-      <c r="M7" s="3" t="b">
+      <c r="L7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M7" s="3"/>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C9" s="7">
+        <v>41296</v>
       </c>
       <c r="D9" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E9" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>41244</v>
+      </c>
+      <c r="I9" s="7">
+        <v>41292</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="7">
         <v>41296</v>
       </c>
-      <c r="E9" s="7">
+      <c r="D10" s="7">
         <v>40817</v>
       </c>
-      <c r="F9" s="7">
+      <c r="E10" s="7">
         <v>41182</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7">
-        <v>41244</v>
-      </c>
-      <c r="J9" s="7">
-        <v>41292</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9">
-        <v>2</v>
-      </c>
-      <c r="M9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E10" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F10" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="3" t="b">
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H10" s="7">
+        <v>41000</v>
+      </c>
       <c r="I10" s="7">
-        <v>41000</v>
-      </c>
-      <c r="J10" s="7">
         <v>41264</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10">
+      <c r="J10" s="7"/>
+      <c r="K10">
         <v>4</v>
       </c>
-      <c r="M10" s="3" t="b">
+      <c r="L10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7">
+        <v>41296</v>
+      </c>
+      <c r="D12" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E12" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>41214</v>
+      </c>
+      <c r="I12" s="7">
+        <v>41292</v>
+      </c>
+      <c r="J12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7">
+        <v>41296</v>
+      </c>
+      <c r="D13" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E13" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>41000</v>
+      </c>
+      <c r="I13" s="7">
+        <v>41203</v>
+      </c>
+      <c r="J13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C15" s="7">
+        <v>41322</v>
+      </c>
+      <c r="D15" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E15" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="7">
+        <v>41000</v>
+      </c>
+      <c r="I15" s="7">
+        <v>41197</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C16" s="7">
+        <v>41322</v>
+      </c>
+      <c r="D16" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E16" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="7">
+        <v>41101</v>
+      </c>
+      <c r="I16" s="7">
+        <v>41307</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7">
+      <c r="C19" s="7">
         <v>41296</v>
       </c>
-      <c r="E12" s="7">
+      <c r="D19" s="7">
         <v>40817</v>
       </c>
-      <c r="F12" s="7">
+      <c r="E19" s="7">
         <v>41182</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7">
         <v>41214</v>
       </c>
-      <c r="J12" s="7">
+      <c r="I19" s="7">
         <v>41292</v>
       </c>
-      <c r="K12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="J19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19">
         <v>4</v>
       </c>
-      <c r="M12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="L19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="7">
         <v>41296</v>
       </c>
-      <c r="E13" s="7">
+      <c r="D20" s="7">
         <v>40817</v>
       </c>
-      <c r="F13" s="7">
+      <c r="E20" s="7">
         <v>41182</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="F20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
         <v>41000</v>
       </c>
-      <c r="J13" s="7">
+      <c r="I20" s="7">
         <v>41203</v>
       </c>
-      <c r="K13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-      <c r="M13" s="3" t="b">
+      <c r="J20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>22</v>
+      </c>
+      <c r="L20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="7">
+        <v>41296</v>
+      </c>
+      <c r="D21" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E21" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>40831</v>
+      </c>
+      <c r="I21" s="7">
+        <v>40923</v>
+      </c>
+      <c r="J21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="7">
+        <v>41296</v>
+      </c>
+      <c r="D22" s="7">
+        <v>40817</v>
+      </c>
+      <c r="E22" s="7">
+        <v>41182</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
+        <v>40466</v>
+      </c>
+      <c r="I22" s="7">
+        <v>40923</v>
+      </c>
+      <c r="J22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E16" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F16" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
-        <v>41214</v>
-      </c>
-      <c r="J16" s="7">
-        <v>41292</v>
-      </c>
-      <c r="K16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-      <c r="M16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E17" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F17" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7">
-        <v>41000</v>
-      </c>
-      <c r="J17" s="7">
-        <v>41203</v>
-      </c>
-      <c r="K17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>22</v>
-      </c>
-      <c r="M17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E18" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F18" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="7">
-        <v>40831</v>
-      </c>
-      <c r="J18" s="7">
-        <v>40923</v>
-      </c>
-      <c r="K18" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="M18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="7">
-        <v>41296</v>
-      </c>
-      <c r="E19" s="7">
-        <v>40817</v>
-      </c>
-      <c r="F19" s="7">
-        <v>41182</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7">
-        <v>40466</v>
-      </c>
-      <c r="J19" s="7">
-        <v>40923</v>
-      </c>
-      <c r="K19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>4</v>
-      </c>
-      <c r="M19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N19" s="3"/>
+      <c r="M22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor changes for demo
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,18 +125,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
-  <si>
-    <t>Scenario</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>S001</t>
   </si>
   <si>
     <t>Employer</t>
-  </si>
-  <si>
-    <t>Sams</t>
   </si>
   <si>
     <t>Employment
@@ -167,19 +161,10 @@
 Not Worked</t>
   </si>
   <si>
-    <t>S002</t>
-  </si>
-  <si>
     <t>Adj</t>
   </si>
   <si>
     <t>QUAL</t>
-  </si>
-  <si>
-    <t>DISQ</t>
-  </si>
-  <si>
-    <t>S006</t>
   </si>
   <si>
     <t>Loews</t>
@@ -224,6 +209,18 @@
     <t>Asserted or Effective
 Process
 Date</t>
+  </si>
+  <si>
+    <t>Freds bar</t>
+  </si>
+  <si>
+    <t>Sids bar</t>
+  </si>
+  <si>
+    <t>S026a</t>
+  </si>
+  <si>
+    <t>Scenario XDS</t>
   </si>
 </sst>
 </file>
@@ -608,469 +605,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N22"/>
+  <dimension ref="B1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" customWidth="1"/>
+    <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="9" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" customWidth="1"/>
-    <col min="13" max="13" width="7" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="5.88671875" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="2"/>
+    <row r="1" spans="2:17" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="2:17" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="Q3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
         <v>41296</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>40817</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>41182</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>41061</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>41292</v>
       </c>
-      <c r="J5" s="7"/>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="L5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="O5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P5" s="3"/>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="7"/>
+      <c r="F6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="M6" s="7"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7">
         <v>41296</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>40817</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>41182</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>41061</v>
-      </c>
       <c r="I7" s="7">
+        <v>40210</v>
+      </c>
+      <c r="J7" s="7">
+        <v>41000</v>
+      </c>
+      <c r="L7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E8" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F8" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I8" s="7">
+        <v>41030</v>
+      </c>
+      <c r="J8" s="7">
+        <v>41295</v>
+      </c>
+      <c r="L8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="7"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E10" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F10" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I10" s="7">
+        <v>41214</v>
+      </c>
+      <c r="J10" s="7">
         <v>41292</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3"/>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D9" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E9" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>41244</v>
-      </c>
-      <c r="I9" s="7">
-        <v>41292</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D10" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E10" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="7">
-        <v>41000</v>
-      </c>
-      <c r="I10" s="7">
-        <v>41264</v>
-      </c>
-      <c r="J10" s="7"/>
       <c r="K10">
         <v>4</v>
       </c>
       <c r="L10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E11" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F11" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I11" s="7">
+        <v>41000</v>
+      </c>
+      <c r="J11" s="7">
+        <v>41203</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="P11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="7"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="7"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="7"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="7"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="7">
+        <v>41322</v>
+      </c>
+      <c r="E17" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F17" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I17" s="7">
+        <v>41000</v>
+      </c>
+      <c r="J17" s="7">
+        <v>41197</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7">
+        <v>41322</v>
+      </c>
+      <c r="E18" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F18" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I18" s="7">
+        <v>41101</v>
+      </c>
+      <c r="J18" s="7">
+        <v>41307</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="7">
         <v>41296</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E21" s="7">
         <v>40817</v>
       </c>
-      <c r="E12" s="7">
+      <c r="F21" s="7">
         <v>41182</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
+      <c r="I21" s="7">
         <v>41214</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J21" s="7">
         <v>41292</v>
-      </c>
-      <c r="J12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>4</v>
-      </c>
-      <c r="L12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D13" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E13" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7">
-        <v>41000</v>
-      </c>
-      <c r="I13" s="7">
-        <v>41203</v>
-      </c>
-      <c r="J13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>2</v>
-      </c>
-      <c r="L13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="7">
-        <v>41322</v>
-      </c>
-      <c r="D15" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E15" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="7">
-        <v>41000</v>
-      </c>
-      <c r="I15" s="7">
-        <v>41197</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="7">
-        <v>41322</v>
-      </c>
-      <c r="D16" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E16" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="7">
-        <v>41101</v>
-      </c>
-      <c r="I16" s="7">
-        <v>41307</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D19" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E19" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
-        <v>41214</v>
-      </c>
-      <c r="I19" s="7">
-        <v>41292</v>
-      </c>
-      <c r="J19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="L19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D20" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E20" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>41000</v>
-      </c>
-      <c r="I20" s="7">
-        <v>41203</v>
-      </c>
-      <c r="J20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>22</v>
-      </c>
-      <c r="L20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="7">
-        <v>41296</v>
-      </c>
-      <c r="D21" s="7">
-        <v>40817</v>
-      </c>
-      <c r="E21" s="7">
-        <v>41182</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7">
-        <v>40831</v>
-      </c>
-      <c r="I21" s="7">
-        <v>40923</v>
-      </c>
-      <c r="J21" s="7" t="b">
-        <v>0</v>
       </c>
       <c r="K21">
         <v>4</v>
@@ -1078,43 +998,121 @@
       <c r="L21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E22" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F22" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I22" s="7">
+        <v>41000</v>
+      </c>
+      <c r="J22" s="7">
+        <v>41203</v>
+      </c>
+      <c r="K22">
         <v>22</v>
       </c>
-      <c r="C22" s="7">
+      <c r="L22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="7">
         <v>41296</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E23" s="7">
         <v>40817</v>
       </c>
-      <c r="E22" s="7">
+      <c r="F23" s="7">
         <v>41182</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="7">
+      <c r="I23" s="7">
+        <v>40831</v>
+      </c>
+      <c r="J23" s="7">
+        <v>40923</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="7">
+        <v>41296</v>
+      </c>
+      <c r="E24" s="7">
+        <v>40817</v>
+      </c>
+      <c r="F24" s="7">
+        <v>41182</v>
+      </c>
+      <c r="I24" s="7">
         <v>40466</v>
       </c>
-      <c r="I22" s="7">
+      <c r="J24" s="7">
         <v>40923</v>
       </c>
-      <c r="J22" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22">
+      <c r="K24">
         <v>4</v>
       </c>
-      <c r="L22" s="3" t="b">
+      <c r="L24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M22" s="3"/>
+      <c r="P24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed during the demo
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="G3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>S001</t>
   </si>
@@ -221,6 +221,15 @@
   </si>
   <si>
     <t>Scenario XDS</t>
+  </si>
+  <si>
+    <t>S011</t>
+  </si>
+  <si>
+    <t>Recency</t>
+  </si>
+  <si>
+    <t>Bogo's Club</t>
   </si>
 </sst>
 </file>
@@ -605,514 +614,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q24"/>
+  <dimension ref="B1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="9" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" customWidth="1"/>
-    <col min="15" max="15" width="7.5546875" customWidth="1"/>
-    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="10" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="2"/>
+    <row r="1" spans="2:18" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:17" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="2:18" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>41296</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>40817</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>41182</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>41061</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>41292</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>3</v>
       </c>
-      <c r="L5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="O5" s="3" t="b">
+      <c r="M5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="P5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" t="s">
+      <c r="Q5" s="3"/>
+      <c r="R5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="7"/>
-      <c r="O6" s="3"/>
+      <c r="K6" s="7"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="7"/>
       <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>41296</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>40817</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>41182</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>40210</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="7">
         <v>41000</v>
       </c>
-      <c r="L7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="O7" s="3"/>
+      <c r="M7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>41296</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>40817</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>41182</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>41030</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>41295</v>
       </c>
-      <c r="L8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="O8" s="3"/>
+      <c r="M8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7"/>
       <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="7"/>
-      <c r="O9" s="3"/>
+      <c r="K9" s="7"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="7"/>
       <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>41296</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <v>40817</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>41182</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>41214</v>
       </c>
-      <c r="J10" s="7">
+      <c r="K10" s="7">
         <v>41292</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>4</v>
       </c>
-      <c r="L10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3" t="s">
+      <c r="M10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>41296</v>
       </c>
-      <c r="E11" s="7">
+      <c r="F11" s="7">
         <v>40817</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>41182</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>41000</v>
       </c>
-      <c r="J11" s="7">
+      <c r="K11" s="7">
         <v>41203</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2</v>
       </c>
-      <c r="L11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="b">
+      <c r="M11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="G12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="7"/>
-      <c r="O12" s="3"/>
+      <c r="K12" s="7"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="7"/>
       <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7">
+        <v>41296</v>
+      </c>
+      <c r="F13" s="7">
+        <v>40817</v>
+      </c>
+      <c r="G13" s="7">
+        <v>41182</v>
+      </c>
       <c r="J13" s="7"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="7"/>
-      <c r="O13" s="3"/>
+      <c r="K13" s="7"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="7"/>
       <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="7"/>
-      <c r="O14" s="3"/>
+      <c r="K14" s="7"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="7"/>
       <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="7"/>
-      <c r="O15" s="3"/>
+      <c r="K15" s="7"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="7"/>
       <c r="P15" s="3"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C17" s="3" t="s">
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="7">
         <v>41322</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="7">
         <v>40817</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="7">
         <v>41182</v>
       </c>
-      <c r="I17" s="7">
+      <c r="J17" s="7">
         <v>41000</v>
       </c>
-      <c r="J17" s="7">
+      <c r="K17" s="7">
         <v>41197</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="M17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="s">
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E18" s="7">
         <v>41322</v>
       </c>
-      <c r="E18" s="7">
+      <c r="F18" s="7">
         <v>40817</v>
       </c>
-      <c r="F18" s="7">
+      <c r="G18" s="7">
         <v>41182</v>
       </c>
-      <c r="I18" s="7">
+      <c r="J18" s="7">
         <v>41101</v>
       </c>
-      <c r="J18" s="7">
+      <c r="K18" s="7">
         <v>41307</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>3</v>
       </c>
-      <c r="M18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="7">
+      <c r="E21" s="7">
         <v>41296</v>
       </c>
-      <c r="E21" s="7">
+      <c r="F21" s="7">
         <v>40817</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="7">
         <v>41182</v>
       </c>
-      <c r="I21" s="7">
+      <c r="J21" s="7">
         <v>41214</v>
       </c>
-      <c r="J21" s="7">
+      <c r="K21" s="7">
         <v>41292</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>4</v>
       </c>
-      <c r="L21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E22" s="7">
         <v>41296</v>
       </c>
-      <c r="E22" s="7">
+      <c r="F22" s="7">
         <v>40817</v>
       </c>
-      <c r="F22" s="7">
+      <c r="G22" s="7">
         <v>41182</v>
       </c>
-      <c r="I22" s="7">
+      <c r="J22" s="7">
         <v>41000</v>
       </c>
-      <c r="J22" s="7">
+      <c r="K22" s="7">
         <v>41203</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>22</v>
       </c>
-      <c r="L22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>41296</v>
       </c>
-      <c r="E23" s="7">
+      <c r="F23" s="7">
         <v>40817</v>
       </c>
-      <c r="F23" s="7">
+      <c r="G23" s="7">
         <v>41182</v>
       </c>
-      <c r="I23" s="7">
+      <c r="J23" s="7">
         <v>40831</v>
       </c>
-      <c r="J23" s="7">
+      <c r="K23" s="7">
         <v>40923</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>4</v>
       </c>
-      <c r="L23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M23" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="7">
+      <c r="E24" s="7">
         <v>41296</v>
       </c>
-      <c r="E24" s="7">
+      <c r="F24" s="7">
         <v>40817</v>
       </c>
-      <c r="F24" s="7">
+      <c r="G24" s="7">
         <v>41182</v>
       </c>
-      <c r="I24" s="7">
+      <c r="J24" s="7">
         <v>40466</v>
       </c>
-      <c r="J24" s="7">
+      <c r="K24" s="7">
         <v>40923</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>4</v>
       </c>
-      <c r="L24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3" t="b">
+      <c r="M24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
syncing my version of working demo
</commit_message>
<xml_diff>
--- a/ky_fpr/TestCases/FPR_TestData.xlsx
+++ b/ky_fpr/TestCases/FPR_TestData.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Demo" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -124,8 +123,117 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maps to the Truth Table ID
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Asserted Override Date
+Enables a consistent result as time passes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Base Period Start Date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Base Period End Date
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>S001</t>
   </si>
@@ -237,6 +345,39 @@
   </si>
   <si>
     <t>Harry's Bar</t>
+  </si>
+  <si>
+    <t>Demo01</t>
+  </si>
+  <si>
+    <t>Demo02</t>
+  </si>
+  <si>
+    <t>2011-20-01</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Demo03</t>
+  </si>
+  <si>
+    <t>Lowes</t>
+  </si>
+  <si>
+    <t>Kohl's</t>
+  </si>
+  <si>
+    <t>RCE</t>
+  </si>
+  <si>
+    <t>BPTW</t>
+  </si>
+  <si>
+    <t>CNCT</t>
+  </si>
+  <si>
+    <t>Demo04</t>
   </si>
 </sst>
 </file>
@@ -244,7 +385,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -321,13 +462,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -634,10 +775,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1776" topLeftCell="A9" activePane="bottomLeft"/>
-      <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1800" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection sqref="A1:P1"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +787,7 @@
     <col min="5" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
     <col min="10" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
     <col min="14" max="14" width="5.88671875" customWidth="1"/>
     <col min="16" max="16" width="9.5546875" customWidth="1"/>
@@ -1271,25 +1412,335 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2304" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>40369</v>
+      </c>
+      <c r="J3" s="6">
+        <v>41334</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <v>40369</v>
+      </c>
+      <c r="J5" s="6">
+        <v>40969</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>41070</v>
+      </c>
+      <c r="J6" s="6">
+        <v>41334</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>40369</v>
+      </c>
+      <c r="J8" s="6">
+        <v>40969</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <v>41153</v>
+      </c>
+      <c r="J9" s="6">
+        <v>41334</v>
+      </c>
+      <c r="K9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>40369</v>
+      </c>
+      <c r="J11" s="6">
+        <v>40969</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>41000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>41289</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6">
+        <v>41336</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="6">
+        <v>41182</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <v>41279</v>
+      </c>
+      <c r="J13" s="6">
+        <v>41334</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>